<commit_message>
modify the workflow and res
</commit_message>
<xml_diff>
--- a/123_convert_xlsx.xlsx
+++ b/123_convert_xlsx.xlsx
@@ -126,34 +126,28 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="B2">
-        <v>262028</v>
+        <v>238385</v>
       </c>
       <c r="C2">
-        <v>340189</v>
+        <v>41727</v>
       </c>
       <c r="D2">
-        <v>396133</v>
+        <v>341388</v>
       </c>
       <c r="E2">
-        <v>445202</v>
+        <v>381541</v>
       </c>
       <c r="F2">
-        <v>267996</v>
+        <v>426050</v>
       </c>
       <c r="G2">
-        <v>413048</v>
+        <v>406224</v>
       </c>
       <c r="H2">
-        <v>525942</v>
-      </c>
-      <c r="I2">
-        <v>415767</v>
-      </c>
-      <c r="J2">
-        <v>416614</v>
+        <v>501930</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -199,34 +193,28 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>1024</v>
+        <v>256</v>
       </c>
       <c r="B5">
-        <v>350832</v>
+        <v>390846</v>
       </c>
       <c r="C5">
-        <v>632056</v>
+        <v>665175</v>
       </c>
       <c r="D5">
-        <v>822597</v>
+        <v>63008</v>
       </c>
       <c r="E5">
-        <v>945565</v>
+        <v>920700</v>
       </c>
       <c r="F5">
-        <v>1029172</v>
+        <v>853379</v>
       </c>
       <c r="G5">
-        <v>1162302</v>
+        <v>810234</v>
       </c>
       <c r="H5">
-        <v>1140391</v>
-      </c>
-      <c r="I5">
-        <v>1207732</v>
-      </c>
-      <c r="J5">
-        <v>664113</v>
+        <v>815155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>